<commit_message>
Indicadores Plano de Trabalho Junho 23
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Alergias/CargaOCLAlergias/CargaAbsentAndUnknownDataUvIps.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Alergias/CargaOCLAlergias/CargaAbsentAndUnknownDataUvIps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Entregaveis/1.RepositorioSemantico/Alergias/CargaOCLAlergias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{453E8507-0BC5-BC40-BE2D-FA3E6BA9E322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842F5418-AF6D-B145-896C-D998B9046638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2300" yWindow="2320" windowWidth="26840" windowHeight="15940" xr2:uid="{C4EBC3E4-7157-504A-9CCD-7D070CBE4E6A}"/>
   </bookViews>
@@ -558,7 +558,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" customWidth="1"/>
     <col min="3" max="3" width="88.1640625" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
   </cols>

</xml_diff>